<commit_message>
- add new indicator.
</commit_message>
<xml_diff>
--- a/DBCrawler/media/Indicator.xlsx
+++ b/DBCrawler/media/Indicator.xlsx
@@ -16,13 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
-  <si>
-    <t>CPI</t>
-  </si>
-  <si>
-    <t>GDP</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t>结汇</t>
   </si>
@@ -144,9 +138,6 @@
     <t>地铁里程</t>
   </si>
   <si>
-    <t>网民数量</t>
-  </si>
-  <si>
     <t>宽带网速</t>
   </si>
   <si>
@@ -261,24 +252,6 @@
     <t>大小非解禁</t>
   </si>
   <si>
-    <t>A股开户</t>
-  </si>
-  <si>
-    <t>B股开户</t>
-  </si>
-  <si>
-    <t>A股活跃账户</t>
-  </si>
-  <si>
-    <t>A股持仓账户</t>
-  </si>
-  <si>
-    <t>A股总帐户</t>
-  </si>
-  <si>
-    <t>B股总账户</t>
-  </si>
-  <si>
     <t>行业从业人数</t>
   </si>
   <si>
@@ -288,9 +261,6 @@
     <t>网上电子支付额</t>
   </si>
   <si>
-    <t>移动上网网民</t>
-  </si>
-  <si>
     <t>地方债数据</t>
   </si>
   <si>
@@ -321,13 +291,22 @@
     <t>汽车品牌4S门店数量</t>
   </si>
   <si>
+    <t>犯罪率排行</t>
+  </si>
+  <si>
+    <t>国债</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>互联网网民数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>各大网站新闻客户端下载量</t>
-  </si>
-  <si>
-    <t>犯罪率排行</t>
-  </si>
-  <si>
-    <t>国债</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>移动网网民数量</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -674,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A105"/>
+  <dimension ref="A2:A97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -687,17 +666,17 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
@@ -892,317 +871,277 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>40</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A69" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A70" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A76" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A77" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A78" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A79" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A80" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A81" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A84" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A86" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A87" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A88" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A89" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A90" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A91" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A92" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A95" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A96" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A97" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A98" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A99" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A100" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A101" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A102" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A103" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A104" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A105" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>